<commit_message>
casos de prueba 15 Settings update
</commit_message>
<xml_diff>
--- a/cypress/downloads/Export.xlsx
+++ b/cypress/downloads/Export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17" count="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18" count="31">
   <si>
     <t>CreatedAtUtc</t>
   </si>
@@ -53,16 +53,19 @@
     <t>SelectedCompany</t>
   </si>
   <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Default Company, LLC.</t>
+  </si>
+  <si>
     <t>Administrator</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Internal</t>
-  </si>
-  <si>
-    <t>Default Company, LLC.</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="n" s="2">
-        <v>45380.98336805555</v>
+        <v>45620.552349537036</v>
       </c>
       <c r="B2" t="s" s="3">
         <v>13</v>
@@ -538,15 +541,56 @@
         <v>15</v>
       </c>
       <c r="J2" t="b" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="b" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="b" s="13">
         <v>0</v>
       </c>
       <c r="M2" t="s" s="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="n" s="2">
+        <v>45380.98336805555</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="J3" t="b" s="11">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b" s="13">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s" s="14">
         <v>16</v>
       </c>
     </row>

</xml_diff>